<commit_message>
Registro de tiempos y comienzo de implementación de CU registrar mensualidad
Se comezó el CU para que el maestro registre la mensualidad de algún alumno
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
+++ b/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98EAD45-134E-4461-881D-6000019DFA6A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8046AF-6304-4689-B5FD-5E31E5A55C95}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,10 +882,10 @@
   <dimension ref="B1:BB28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="AS9" sqref="AS9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,36 +1941,40 @@
         <v>15</v>
       </c>
       <c r="AN14" s="23"/>
-      <c r="AO14" s="23"/>
+      <c r="AO14" s="23">
+        <v>3</v>
+      </c>
       <c r="AP14" s="23">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AQ14" s="23"/>
-      <c r="AR14" s="23"/>
+      <c r="AR14" s="23">
+        <v>4</v>
+      </c>
       <c r="AS14" s="23">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AT14" s="23"/>
       <c r="AU14" s="23"/>
       <c r="AV14" s="23">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AW14" s="23"/>
       <c r="AX14" s="23"/>
       <c r="AY14" s="23">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="AZ14" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BA14" s="36">
         <f>G14-AZ14</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="BB14" s="2"/>
     </row>
@@ -2146,7 +2150,7 @@
       <c r="AZ16" s="31"/>
       <c r="BA16" s="31"/>
     </row>
-    <row r="17" spans="2:54" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:54" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="34"/>
       <c r="C17" s="29"/>
       <c r="D17" s="28" t="s">
@@ -2433,7 +2437,7 @@
       <c r="BA19" s="36"/>
       <c r="BB19" s="2"/>
     </row>
-    <row r="20" spans="2:54" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:54" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="34"/>
       <c r="C20" s="29"/>
       <c r="D20" s="28" t="s">
@@ -2547,7 +2551,7 @@
       </c>
       <c r="BB20" s="2"/>
     </row>
-    <row r="21" spans="2:54" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:54" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="34"/>
       <c r="C21" s="29"/>
       <c r="D21" s="28" t="s">
@@ -3291,11 +3295,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3307,6 +3306,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Registo de tiempos y creación del Diagrama de paquetes
Se registraron los tiempos empleados en la codificación y realización del Diagrama de paquetes, se modifico el Plan de pruebas, y se agregó la imagen del Diagrama de pruebas dejando pendiente solo la implementación de las pruebas unitarias
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
+++ b/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8046AF-6304-4689-B5FD-5E31E5A55C95}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41056057-69BA-401C-BF84-9E1375376C76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="64">
   <si>
     <t>Columna</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>CU-21</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -882,10 +885,10 @@
   <dimension ref="B1:BB28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AL18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AS9" sqref="AS9"/>
+      <selection pane="bottomRight" activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,7 +1414,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G9" s="18">
         <v>1.5</v>
@@ -1494,24 +1497,26 @@
         <v>1.5</v>
       </c>
       <c r="AT9" s="15"/>
-      <c r="AU9" s="14"/>
+      <c r="AU9" s="14">
+        <v>2</v>
+      </c>
       <c r="AV9" s="14">
         <f t="shared" si="13"/>
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AW9" s="15"/>
       <c r="AX9" s="14"/>
       <c r="AY9" s="14">
         <f>AV9-AX9</f>
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ9" s="36">
         <f t="shared" ref="AZ9:AZ27" si="14">H9+K9+N9+Q9+T9+W9+Z9+AC9+AF9+AI9+AL9+AO9+AR9+AU9+AX9</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA9" s="36">
         <f>G9-AZ9</f>
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="10" spans="2:54" s="25" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2734,7 +2739,7 @@
         <v>42</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G23" s="44">
         <v>15</v>
@@ -2811,30 +2816,32 @@
         <v>15</v>
       </c>
       <c r="AQ23" s="40"/>
-      <c r="AR23" s="40"/>
+      <c r="AR23" s="40">
+        <v>3</v>
+      </c>
       <c r="AS23" s="40">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AT23" s="40"/>
       <c r="AU23" s="40"/>
       <c r="AV23" s="40">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AW23" s="40"/>
       <c r="AX23" s="40"/>
       <c r="AY23" s="40">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AZ23" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA23" s="36">
         <f>G23-AZ23</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="BB23" s="2"/>
     </row>
@@ -3021,7 +3028,7 @@
         <v>42</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G26" s="44">
         <v>15</v>
@@ -3086,42 +3093,48 @@
         <v>15</v>
       </c>
       <c r="AK26" s="40"/>
-      <c r="AL26" s="40"/>
+      <c r="AL26" s="40">
+        <v>2</v>
+      </c>
       <c r="AM26" s="40">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AN26" s="40"/>
-      <c r="AO26" s="40"/>
+      <c r="AO26" s="40">
+        <v>2</v>
+      </c>
       <c r="AP26" s="40">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AQ26" s="40"/>
-      <c r="AR26" s="40"/>
+      <c r="AR26" s="40">
+        <v>2</v>
+      </c>
       <c r="AS26" s="40">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AT26" s="40"/>
       <c r="AU26" s="40"/>
       <c r="AV26" s="40">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AW26" s="40"/>
       <c r="AX26" s="40"/>
       <c r="AY26" s="40">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AZ26" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA26" s="36">
         <f>G26-AZ26</f>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="BB26" s="2"/>
     </row>
@@ -3295,6 +3308,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3306,11 +3324,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Termino de CU Registrar mensualidad
Se concluyó con la implementación del CU en el que el maestro registra la mensualidad del alumno.
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
+++ b/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41056057-69BA-401C-BF84-9E1375376C76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E539374A-92A2-444E-A4AC-EFBA407E6D78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -885,10 +885,10 @@
   <dimension ref="B1:BB28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AL18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AJ9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AR26" sqref="AR26"/>
+      <selection pane="bottomRight" activeCell="AX11" sqref="AX11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1588,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G11" s="27">
         <v>15</v>
@@ -1671,24 +1671,28 @@
         <v>15</v>
       </c>
       <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
+      <c r="AU11" s="23">
+        <v>8</v>
+      </c>
       <c r="AV11" s="23">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="AW11" s="23"/>
-      <c r="AX11" s="23"/>
+      <c r="AX11" s="23">
+        <v>2</v>
+      </c>
       <c r="AY11" s="23">
         <f>AV11-AX11</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="AZ11" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA11" s="36">
         <f>G11-AZ11</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="BB11" s="2"/>
     </row>
@@ -1875,7 +1879,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G14" s="27">
         <v>15</v>
@@ -3308,11 +3312,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3324,6 +3323,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Pruebas Unitarias, registros de tiempos y modificaciones
Se agregaron las pruebas unitarias de los métodos correspondientes a PagoMaestro y Maestro, así como el registro de los tiempos y unas modificaciones pequeñas en el código para validación de algunos campos
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
+++ b/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0EFE24-1B18-41A8-A255-7D3D148F2068}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD555065-440D-4DE5-90A2-6F00DC6D4410}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -524,7 +524,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -885,10 +884,10 @@
   <dimension ref="B1:BB28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AQ11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AZ17" sqref="AZ17"/>
+      <selection pane="bottomRight" activeCell="F23" activeCellId="1" sqref="F24 F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,84 +969,84 @@
       <c r="BA3" s="2"/>
     </row>
     <row r="4" spans="2:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="53"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="53"/>
+      <c r="O4" s="52"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="53"/>
+      <c r="R4" s="52"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="52" t="s">
+      <c r="T4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="53"/>
+      <c r="U4" s="52"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="52" t="s">
+      <c r="W4" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="53"/>
+      <c r="X4" s="52"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="52" t="s">
+      <c r="Z4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="53"/>
+      <c r="AA4" s="52"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="52" t="s">
+      <c r="AC4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="53"/>
+      <c r="AD4" s="52"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG4" s="53"/>
+      <c r="AF4" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="52"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="52" t="s">
+      <c r="AI4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="53"/>
+      <c r="AJ4" s="52"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="52" t="s">
+      <c r="AL4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="53"/>
+      <c r="AM4" s="52"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="52" t="s">
+      <c r="AO4" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="53"/>
+      <c r="AP4" s="52"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="52" t="s">
+      <c r="AR4" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="53"/>
+      <c r="AS4" s="52"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="52" t="s">
+      <c r="AU4" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="53"/>
+      <c r="AV4" s="52"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="52" t="s">
+      <c r="AX4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="53"/>
-      <c r="AZ4" s="52" t="s">
+      <c r="AY4" s="52"/>
+      <c r="AZ4" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="53"/>
+      <c r="BA4" s="52"/>
     </row>
     <row r="5" spans="2:54" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -2776,7 +2775,7 @@
       <c r="E23" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="43" t="s">
         <v>63</v>
       </c>
       <c r="G23" s="44">
@@ -2892,8 +2891,8 @@
       <c r="E24" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="48" t="s">
-        <v>43</v>
+      <c r="F24" s="43" t="s">
+        <v>63</v>
       </c>
       <c r="G24" s="44">
         <v>3</v>
@@ -2982,18 +2981,20 @@
         <v>3</v>
       </c>
       <c r="AW24" s="40"/>
-      <c r="AX24" s="40"/>
+      <c r="AX24" s="40">
+        <v>1</v>
+      </c>
       <c r="AY24" s="40">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ24" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA24" s="36">
         <f>G24-AZ24</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BB24" s="2"/>
     </row>
@@ -3186,7 +3187,7 @@
         <v>42</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="G27" s="44">
         <v>3</v>
@@ -3275,28 +3276,30 @@
         <v>3</v>
       </c>
       <c r="AW27" s="40"/>
-      <c r="AX27" s="40"/>
+      <c r="AX27" s="40">
+        <v>1</v>
+      </c>
       <c r="AY27" s="40">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ27" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA27" s="36">
         <f>G27-AZ27</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BB27" s="2"/>
     </row>
     <row r="28" spans="2:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="49"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="50"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="5"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="51"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="15"/>
@@ -3346,11 +3349,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3362,6 +3360,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Pruebas unitarias del Pago de inscripción
Se realizaron las pruebas de unidad para verificar que los pagos se realien correctamente y además que modificaron los tiempos de las plantillas
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
+++ b/Plantillas/Entrega 4/Plantilla Lista de Tareas de la Entrega 3 - copia - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD555065-440D-4DE5-90A2-6F00DC6D4410}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34615D06-89EA-4729-955B-789D325CDBFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="63">
   <si>
     <t>Columna</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>IRVIN VERA</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>IRVIN VERA, ISRAEL OZUNA, RENATO VARGAS</t>
@@ -884,10 +881,10 @@
   <dimension ref="B1:BB28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AS6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F23" activeCellId="1" sqref="F24 F23"/>
+      <selection pane="bottomRight" activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1178,7 @@
     <row r="6" spans="2:54" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="C6" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1238,13 +1235,13 @@
       <c r="B7" s="18"/>
       <c r="C7" s="12"/>
       <c r="D7" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="G7" s="18">
         <v>2</v>
@@ -1352,7 +1349,7 @@
     <row r="8" spans="2:54" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="14"/>
@@ -1409,13 +1406,13 @@
       <c r="B9" s="18"/>
       <c r="C9" s="12"/>
       <c r="D9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="18">
         <v>1.5</v>
@@ -1522,10 +1519,10 @@
     </row>
     <row r="10" spans="2:54" s="25" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -1583,13 +1580,13 @@
       <c r="B11" s="26"/>
       <c r="C11" s="21"/>
       <c r="D11" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="47" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="27">
         <v>15</v>
@@ -1701,13 +1698,13 @@
       <c r="B12" s="26"/>
       <c r="C12" s="21"/>
       <c r="D12" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="47" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="G12" s="27">
         <v>3</v>
@@ -1796,27 +1793,29 @@
         <v>3</v>
       </c>
       <c r="AW12" s="23"/>
-      <c r="AX12" s="23"/>
+      <c r="AX12" s="23">
+        <v>1</v>
+      </c>
       <c r="AY12" s="23">
         <f t="shared" ref="AY12:AY27" si="15">AV12-AX12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ12" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA12" s="36">
         <f>G12-AZ12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BB12" s="2"/>
     </row>
     <row r="13" spans="2:54" s="25" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -1874,13 +1873,13 @@
       <c r="B14" s="26"/>
       <c r="C14" s="21"/>
       <c r="D14" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="47" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="27">
         <v>15</v>
@@ -1992,13 +1991,13 @@
       <c r="B15" s="26"/>
       <c r="C15" s="21"/>
       <c r="D15" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="47" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="G15" s="27">
         <v>3</v>
@@ -2087,27 +2086,29 @@
         <v>3</v>
       </c>
       <c r="AW15" s="23"/>
-      <c r="AX15" s="23"/>
+      <c r="AX15" s="23">
+        <v>1</v>
+      </c>
       <c r="AY15" s="23">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ15" s="36">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA15" s="36">
         <f>G15-AZ15</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BB15" s="2"/>
     </row>
     <row r="16" spans="2:54" s="33" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
@@ -2164,13 +2165,13 @@
       <c r="B17" s="34"/>
       <c r="C17" s="29"/>
       <c r="D17" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="35">
         <v>15</v>
@@ -2294,13 +2295,13 @@
       <c r="B18" s="34"/>
       <c r="C18" s="29"/>
       <c r="D18" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="35">
         <v>3</v>
@@ -2408,10 +2409,10 @@
     </row>
     <row r="19" spans="2:54" s="33" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
@@ -2469,13 +2470,13 @@
       <c r="B20" s="34"/>
       <c r="C20" s="29"/>
       <c r="D20" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20" s="35">
         <v>15</v>
@@ -2595,13 +2596,13 @@
       <c r="B21" s="34"/>
       <c r="C21" s="29"/>
       <c r="D21" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G21" s="35">
         <v>3</v>
@@ -2709,10 +2710,10 @@
     </row>
     <row r="22" spans="2:54" s="42" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="38" t="s">
         <v>59</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>60</v>
       </c>
       <c r="D22" s="39"/>
       <c r="E22" s="39"/>
@@ -2770,13 +2771,13 @@
       <c r="B23" s="43"/>
       <c r="C23" s="38"/>
       <c r="D23" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="44">
         <v>15</v>
@@ -2886,13 +2887,13 @@
       <c r="B24" s="43"/>
       <c r="C24" s="38"/>
       <c r="D24" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>42</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G24" s="44">
         <v>3</v>
@@ -3000,10 +3001,10 @@
     </row>
     <row r="25" spans="2:54" s="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="39"/>
       <c r="E25" s="39"/>
@@ -3061,13 +3062,13 @@
       <c r="B26" s="43"/>
       <c r="C26" s="38"/>
       <c r="D26" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>42</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G26" s="44">
         <v>15</v>
@@ -3181,13 +3182,13 @@
       <c r="B27" s="43"/>
       <c r="C27" s="38"/>
       <c r="D27" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G27" s="44">
         <v>3</v>
@@ -3349,6 +3350,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3360,11 +3366,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>